<commit_message>
updated files for H2 databse
</commit_message>
<xml_diff>
--- a/Tax.xlsx
+++ b/Tax.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23801"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24701"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mapradee\OneDrive - Capgemini\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mmani\IdeaProjects\java-tutorials\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7E2151EC-A70B-46AC-8873-2B44CCF2B387}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C2F80857-2702-42BD-91BB-C207970729AB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="9800" xr2:uid="{6068E26E-9D4D-43ED-9A83-749FCA6BEAFF}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{6068E26E-9D4D-43ED-9A83-749FCA6BEAFF}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -24,9 +24,7 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
       </xcalcf:calcFeatures>
     </ext>
@@ -476,24 +474,24 @@
   <dimension ref="A1:J25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+      <selection activeCell="G13" sqref="G13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="13.1796875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.7265625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="13.21875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.77734375" bestFit="1" customWidth="1"/>
     <col min="3" max="4" width="13" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="11.7265625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.77734375" bestFit="1" customWidth="1"/>
     <col min="6" max="8" width="14" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="23.36328125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="12.7265625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="14.453125" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="18.36328125" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="11.7265625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="23.33203125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="12.77734375" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="14.44140625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="18.33203125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="11.77734375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B1" t="s">
         <v>19</v>
       </c>
@@ -501,12 +499,12 @@
         <v>24</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>0</v>
       </c>
       <c r="B2" s="3">
-        <v>2600000</v>
+        <v>1800000</v>
       </c>
       <c r="F2" t="s">
         <v>6</v>
@@ -516,28 +514,28 @@
       </c>
       <c r="J2" s="3">
         <f>B9-D25-C5-C7</f>
-        <v>151185.424</v>
-      </c>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.35">
+        <v>111602.83199999999</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>1</v>
       </c>
       <c r="B3" s="3">
         <f>B2*0.4</f>
-        <v>1040000</v>
+        <v>720000</v>
       </c>
       <c r="D3" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>2</v>
       </c>
       <c r="B4" s="3">
         <f>B3*0.4</f>
-        <v>416000</v>
+        <v>288000</v>
       </c>
       <c r="D4" t="s">
         <v>21</v>
@@ -549,17 +547,17 @@
         <v>50000</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>3</v>
       </c>
       <c r="B5" s="3">
         <f>0.12*B3</f>
-        <v>124800</v>
+        <v>86400</v>
       </c>
       <c r="C5" s="3">
         <f>B5/12</f>
-        <v>10400</v>
+        <v>7200</v>
       </c>
       <c r="D5" t="s">
         <v>20</v>
@@ -571,13 +569,13 @@
         <v>150000</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>4</v>
       </c>
       <c r="B6" s="3">
         <f>0.0481*B3</f>
-        <v>50024</v>
+        <v>34632</v>
       </c>
       <c r="D6" t="s">
         <v>22</v>
@@ -589,7 +587,7 @@
         <v>200000</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>18</v>
       </c>
@@ -602,13 +600,13 @@
       </c>
       <c r="G7" s="3"/>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>5</v>
       </c>
       <c r="B8" s="3">
         <f>(B2-B5-B6)</f>
-        <v>2425176</v>
+        <v>1678968</v>
       </c>
       <c r="C8" t="s">
         <v>23</v>
@@ -621,21 +619,21 @@
         <v>400000</v>
       </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>15</v>
       </c>
       <c r="B9" s="3">
         <f>B8/12</f>
-        <v>202098</v>
-      </c>
-    </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.35">
+        <v>139914</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B12" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B13" s="2">
         <v>0</v>
       </c>
@@ -650,10 +648,10 @@
       </c>
       <c r="G13" s="3">
         <f>B8-G8</f>
-        <v>2025176</v>
-      </c>
-    </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.35">
+        <v>1278968</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B14" s="2">
         <v>250001</v>
       </c>
@@ -669,7 +667,7 @@
       </c>
       <c r="H14" s="5"/>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B15" s="2">
         <v>500001</v>
       </c>
@@ -684,7 +682,7 @@
         <v>25000</v>
       </c>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B16" s="2">
         <v>750001</v>
       </c>
@@ -700,7 +698,7 @@
       </c>
       <c r="I16" s="3"/>
     </row>
-    <row r="17" spans="2:10" x14ac:dyDescent="0.35">
+    <row r="17" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B17" s="2">
         <v>1000000</v>
       </c>
@@ -716,7 +714,7 @@
       </c>
       <c r="I17" s="3"/>
     </row>
-    <row r="18" spans="2:10" x14ac:dyDescent="0.35">
+    <row r="18" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B18" s="2">
         <v>1250000</v>
       </c>
@@ -731,7 +729,7 @@
         <v>62500</v>
       </c>
     </row>
-    <row r="19" spans="2:10" x14ac:dyDescent="0.35">
+    <row r="19" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B19" s="2">
         <v>1500001</v>
       </c>
@@ -741,50 +739,50 @@
       </c>
       <c r="E19" s="3">
         <f>IF((IF(B8&gt;1500000,(B8-1500000)*0.3,0))&gt;0,(IF(B8&gt;1500000,(B8-1500000)*0.3,0)),0)</f>
-        <v>277552.8</v>
-      </c>
-    </row>
-    <row r="20" spans="2:10" x14ac:dyDescent="0.35">
+        <v>53690.400000000001</v>
+      </c>
+    </row>
+    <row r="20" spans="2:10" x14ac:dyDescent="0.3">
       <c r="F20" s="2"/>
       <c r="J20" s="3"/>
     </row>
-    <row r="21" spans="2:10" x14ac:dyDescent="0.35">
+    <row r="21" spans="2:10" x14ac:dyDescent="0.3">
       <c r="C21" t="s">
         <v>14</v>
       </c>
       <c r="D21" s="4">
         <f>SUM(E14:E20)</f>
-        <v>465052.8</v>
+        <v>241190.39999999999</v>
       </c>
       <c r="F21" s="2"/>
     </row>
-    <row r="22" spans="2:10" x14ac:dyDescent="0.35">
+    <row r="22" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B22" t="s">
         <v>13</v>
       </c>
       <c r="D22">
         <f>0.04*D21</f>
-        <v>18602.112000000001</v>
+        <v>9647.616</v>
       </c>
       <c r="F22" s="2"/>
       <c r="G22" s="3"/>
     </row>
-    <row r="24" spans="2:10" x14ac:dyDescent="0.35">
+    <row r="24" spans="2:10" x14ac:dyDescent="0.3">
       <c r="C24" t="s">
         <v>16</v>
       </c>
       <c r="D24" s="4">
         <f>D21+D22</f>
-        <v>483654.91200000001</v>
-      </c>
-    </row>
-    <row r="25" spans="2:10" x14ac:dyDescent="0.35">
+        <v>250838.016</v>
+      </c>
+    </row>
+    <row r="25" spans="2:10" x14ac:dyDescent="0.3">
       <c r="C25" t="s">
         <v>17</v>
       </c>
       <c r="D25">
         <f>D24/12</f>
-        <v>40304.576000000001</v>
+        <v>20903.168000000001</v>
       </c>
     </row>
   </sheetData>
@@ -801,7 +799,7 @@
       <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>